<commit_message>
Screen Layout and TestCases
</commit_message>
<xml_diff>
--- a/Dokumentation/ProductBacklog.xlsx
+++ b/Dokumentation/ProductBacklog.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="PB" sheetId="1" r:id="rId1"/>
     <sheet name="Festwerte" sheetId="2" r:id="rId2"/>
+    <sheet name="Ticket" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Kano">Festwerte!$D$2:$D$8</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="246">
   <si>
     <t>ID</t>
   </si>
@@ -696,6 +697,126 @@
   <si>
     <t>Display Strategy
 Corporate Design</t>
+  </si>
+  <si>
+    <t>Session Handling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concept for Session handling </t>
+  </si>
+  <si>
+    <t>Documentation available</t>
+  </si>
+  <si>
+    <t>Advanced Database concept</t>
+  </si>
+  <si>
+    <t>Specification on how the dataflow between the local and a possible internet database could be realized</t>
+  </si>
+  <si>
+    <t>Build Display Strategy for Small Mobiles</t>
+  </si>
+  <si>
+    <t>Small Layouts for all views must be implemented</t>
+  </si>
+  <si>
+    <t>Layouts 
+- activityEdit.xml
+- activityLoginRegister.xml
+- activityMain.xml
+- activityReports.xml
+- report_fragment_category_summary.xml
+- report_fragment_shop_summary.xml
+available and developer tested.</t>
+  </si>
+  <si>
+    <t>Build Display Strategy for Large Mobiles</t>
+  </si>
+  <si>
+    <t>Large Layouts for all views must be implemented</t>
+  </si>
+  <si>
+    <t>Build Display Strategy for Xlarge Mobiles (Tablets)</t>
+  </si>
+  <si>
+    <t>Xlarge Layouts for all views must be implemented</t>
+  </si>
+  <si>
+    <t>activityEdit.xml
+activityLoginRegister.xml
+activityMain.xml
+activityReports.xml
+report_fragment_category_summary.xml
+report_fragment_shop_summary.xml</t>
+  </si>
+  <si>
+    <t>ID(in GIT)</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview not scaled right in Emulator </t>
+  </si>
+  <si>
+    <t>Technical Component</t>
+  </si>
+  <si>
+    <t>MainActivity/Controller</t>
+  </si>
+  <si>
+    <t>Sum not displayed in overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu not implemented </t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Error when Camera opens, libwvm.so failed to open</t>
+  </si>
+  <si>
+    <t>CameraView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onPollAlarm problem </t>
+  </si>
+  <si>
+    <t>Spinner error</t>
+  </si>
+  <si>
+    <t>EditActivity/Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double entries </t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Testsupport</t>
+  </si>
+  <si>
+    <t>Screenflow</t>
+  </si>
+  <si>
+    <t>Regarding codereview collect locally possibilities (wihtin code) for refactoring</t>
+  </si>
+  <si>
+    <t>Local List available</t>
+  </si>
+  <si>
+    <t>Additional general tests supporting tests. I.E. evaluate Android Monitor</t>
+  </si>
+  <si>
+    <t>Git Issues created</t>
+  </si>
+  <si>
+    <t>Additional Screenflow Requirements regarding Return Button</t>
+  </si>
+  <si>
+    <t>Return button behaves correct…</t>
   </si>
 </sst>
 </file>
@@ -1056,13 +1177,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1193,7 @@
     <col min="4" max="4" width="38.140625" customWidth="1"/>
     <col min="5" max="5" width="45.42578125" customWidth="1"/>
     <col min="6" max="6" width="38.140625" customWidth="1"/>
-    <col min="13" max="13" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2101,7 +2222,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2650,7 +2771,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3117,7 +3238,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -4036,7 +4157,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -4072,7 +4193,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -4108,7 +4229,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -4144,7 +4265,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -4180,23 +4301,300 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>84</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="F85" s="2"/>
+      <c r="G85">
+        <v>5</v>
+      </c>
+      <c r="H85" t="s">
+        <v>15</v>
+      </c>
+      <c r="I85">
+        <v>5</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85" t="s">
+        <v>20</v>
+      </c>
+      <c r="L85" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>85</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="G86">
+        <v>5</v>
+      </c>
+      <c r="H86" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86">
+        <v>20</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+      <c r="K86" t="s">
+        <v>18</v>
+      </c>
+      <c r="L86" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>86</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G87">
+        <v>5</v>
+      </c>
+      <c r="H87" t="s">
+        <v>15</v>
+      </c>
+      <c r="I87">
+        <v>3</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87" t="s">
+        <v>18</v>
+      </c>
+      <c r="L87" t="s">
+        <v>196</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>87</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G88">
+        <v>5</v>
+      </c>
+      <c r="H88" t="s">
+        <v>15</v>
+      </c>
+      <c r="I88">
+        <v>3</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88" t="s">
+        <v>18</v>
+      </c>
+      <c r="L88" t="s">
+        <v>196</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G89">
+        <v>5</v>
+      </c>
+      <c r="H89" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89">
+        <v>3</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89" t="s">
+        <v>18</v>
+      </c>
+      <c r="L89" t="s">
+        <v>196</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B90" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90" t="s">
+        <v>16</v>
+      </c>
+      <c r="I90">
+        <v>5</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90" t="s">
+        <v>21</v>
+      </c>
+      <c r="L90" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B91" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G91">
+        <v>8</v>
+      </c>
+      <c r="H91" t="s">
+        <v>15</v>
+      </c>
+      <c r="I91">
+        <v>3</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+      <c r="K91" t="s">
+        <v>20</v>
+      </c>
+      <c r="L91" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B92" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G92">
+        <v>3</v>
+      </c>
+      <c r="H92" t="s">
+        <v>16</v>
+      </c>
+      <c r="I92">
+        <v>3</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92" t="s">
+        <v>18</v>
+      </c>
+      <c r="L92" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H92">
       <formula1>Moscow</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I92">
       <formula1>Value</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J92">
       <formula1>Risk</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K92">
       <formula1>Kano</formula1>
     </dataValidation>
   </dataValidations>
@@ -4350,4 +4748,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>